<commit_message>
Correção na planilha de Analytics
</commit_message>
<xml_diff>
--- a/documents/xlsx/quartis.xlsx
+++ b/documents/xlsx/quartis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\Iniciativa-0\documents\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakar\Desktop\BandTec\Primeiro semestre\Iniciativa 0\startech\documents\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="11730"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Ideal</t>
   </si>
@@ -35,12 +35,6 @@
     <t>Atenção</t>
   </si>
   <si>
-    <t>Alerta 1</t>
-  </si>
-  <si>
-    <t>18 ºC</t>
-  </si>
-  <si>
     <t>22 ºC</t>
   </si>
   <si>
@@ -50,41 +44,41 @@
     <t>30 ºC</t>
   </si>
   <si>
-    <t>35 ºC</t>
-  </si>
-  <si>
-    <t>Legendas</t>
-  </si>
-  <si>
-    <t>Alerta 2</t>
-  </si>
-  <si>
-    <t>MÍNIMOS</t>
-  </si>
-  <si>
-    <t>1º QUARTIL</t>
-  </si>
-  <si>
-    <t>MEDIANA</t>
-  </si>
-  <si>
-    <t>3º QUARTIL</t>
-  </si>
-  <si>
-    <t>MÁXIMA</t>
-  </si>
-  <si>
     <t>Temperatura ºc</t>
   </si>
   <si>
     <t>Umidade %</t>
+  </si>
+  <si>
+    <t>&lt;= 18 ºC</t>
+  </si>
+  <si>
+    <t>35 ºC =&gt;</t>
+  </si>
+  <si>
+    <t>80% =&gt;</t>
+  </si>
+  <si>
+    <t>&lt;= 25%</t>
+  </si>
+  <si>
+    <t>Alerta 1 Temperatura</t>
+  </si>
+  <si>
+    <t>Alerta 2 Temperatura</t>
+  </si>
+  <si>
+    <t>Alerta 1 Umidade</t>
+  </si>
+  <si>
+    <t>Alerta 2 Umidade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,14 +110,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -211,99 +197,52 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -319,49 +258,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>486360</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>57473</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="647700" y="3086100"/>
-          <a:ext cx="4191585" cy="2314898"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -630,153 +526,112 @@
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="B2" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>10</v>
+      <c r="E3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>8</v>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>10</v>
+      <c r="E7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8">
         <v>0.6</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.5</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>0.35</v>
       </c>
-      <c r="F8" s="11">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="F8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="19"/>
     </row>
     <row r="19" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J19" s="21"/>
+      <c r="J19" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B15:C15"/>
+  <mergeCells count="2">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>